<commit_message>
Refactored question ground truth
</commit_message>
<xml_diff>
--- a/AzureOpenAILogProbs/Images/AzureOpenAILogProbs.xlsx
+++ b/AzureOpenAILogProbs/Images/AzureOpenAILogProbs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bart\source\repos\AzureOpenAILogProbs\AzureOpenAILogProbs\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F91D0F-4F96-45C9-AADD-78F0FA951515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F26ED3-0F34-4D6C-9227-495CFCBBB5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{024B4532-7F17-405B-A065-366127F25B57}"/>
   </bookViews>
@@ -18,12 +18,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$G$9:$G$13</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$9:$H$13</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$G$9:$G$13</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$H$9:$H$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$9:$G$13</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$9:$H$13</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$G$9:$G$13</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$9:$H$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -109,10 +103,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -157,9 +151,28 @@
                 <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:rPr>
+              <a:t>Is there enough information to answer the following question:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:rPr>
               <a:t>Has Steve Cohen been the longest-serving owner of the Mets?</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -1157,7 +1170,7 @@
   <dimension ref="G9:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>